<commit_message>
AI Agent Tool Updated with all the important updates
</commit_message>
<xml_diff>
--- a/data/source_file.xlsx
+++ b/data/source_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukeshkr\Desktop\DefenseExtraction\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukeshkr\Agentic-AI-Defense-Data-Extraction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B2F740-D2FA-41FE-8DC9-3347711234D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80390F9-F97D-4122-AC78-26C9A56B3B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1789C02F-0F05-431D-B1D8-FBD75DE85A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1789C02F-0F05-431D-B1D8-FBD75DE85A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Source URL</t>
   </si>
@@ -47,10 +47,112 @@
     <t>Contract Description</t>
   </si>
   <si>
+    <t>BAE Systems - Norfolk Ship Repair, Norfolk, Virginia, is awarded a $107,736,087, firm-fixed-price contract for the execution of the USS Ross (DDG 71) fiscal 2023 extended dry-docking selected restricted availability. This availability will include a combination of maintenance, modernization and repair of the USS Ross. This contract includes options which, if exercised, would bring the cumulative value of this contract to $123,876,183. Work will be performed in Norfolk, Virginia, and is expected to be completed by March 2024. Fiscal 2022 operations and maintenance (Navy) funds in the amount of $93,897,036 (87%); and fiscal 2022 other procurement (Navy) funds in the amount of $13,839,051 (13%) will be obligated at time of award, of which $93,897,036 will expire at the end of the current fiscal year. This contract was competitively procured using full and open competition via the System for Award Management website. Competitive proposals were received in response to Solicitation Number (N00024-22-R-4422). The Naval Sea Systems Command, Washington, D.C., is the contracting activity (N00024-22-C-4422).</t>
+  </si>
+  <si>
+    <t>The Boeing Co., St. Louis, Missouri, is awarded a $25,648,020 fixed-firm-price, cost-plus-fixed-fee and cost-only, full rate production contract for the production of High-Altitude Anti-Submarine Warfare Weapon Capability Air Launch Accessory equipment, related engineering and hardware repair services, and other direct cost support. This contract includes options, which, if exercised, would bring the cumulative value of this contract to $121,426,700. Work will be performed in St. Charles, Missouri (44%); St. Louis, Missouri (26%); Salt Lake City, Utah (12%); Minneapolis, Minnesota (4%); Joplin, Missouri (2%),; Piedmont, Missouri (2%); Orlando, Florida (2%); Cedar Rapids, Iowa (2%); Chandler, Arizona (1%); Berea, Ohio (1%); Wichita, Kansas (1%); Albuquerque, New Mexico (1%); Lexington, Kentucky, (1%); and Chatsworth, California (1%), and is expected to be completed by September 2024. If all options are exercised, work will continue through September 2030. Fiscal 2020 weapons procurement (Navy) funds in the amount of $11,535,520 (98%); and fiscal 2021 weapons procurement (Navy) funds in the amount of $279,074 (2%) funding will be obligated at time of award, of which $11,535,520 will expire at the end of the current fiscal year. This contract was not competitively procured in accordance with 10 U.S. Code 2304(c) (1) — only one responsible source and no other supplies or services will satisfy agency requirements. The Naval Sea Systems Command, Washington, D.C., is the contracting activity (N00024-22-C-6407).</t>
+  </si>
+  <si>
+    <t>Intermat,* Biddeford, Maine, is awarded a $17,736,279 firm-fixed-price, cost-plus-fixed-fee, and cost-only indefinite-delivery/indefinite-quantity contract for the delivery of Submarine Launched Ballistic Missile nose-tip materials. This contract does not include options. This contract combines purchases for the Navy (82.23%) and the government of the United Kingdom (17.77%) under the Foreign Military Sales program. Work will be performed in Biddeford, Maine, and is expected to be completed by July 2027. Fiscal 2022 Weapons Procurement (Navy) funds in the amount of $1,301,611 will be obligated at time of award. This contract was not competitively procured in accordance with 10 U.S. Code 2304(c)(1) [now 10 U.S. Code 3204(a)(1)] — only one responsible source and no other type of supplies or services will satisfy agency requirements. The Naval Surface Warfare Center Dahlgren Division, Dahlgren, Virginia, is the contracting activity (N0017822D4404).</t>
+  </si>
+  <si>
+    <t>Raytheon Co., Tewksbury, Massachusetts, is awarded an $11,172,229 firm-fixed-price modification to previously awarded contract N00024-22-C-5522 for Total Ship Computing Environment Lab hardware for modernization/technical refresh and Conventional Prompt Strike to support DDG 1000-class combat system activation, sustainment and modernization.  Work will be performed in Nashua, New Hampshire (92%); Portsmouth, Rhode Island (4%); and  Tewksbury, Massachusetts (4%), and is expected to be completed by November 2023. Fiscal 2022 other procurement (Navy) funds in the amount of $9,333,203 (84%); and fiscal 2022 research, development, test and evaluation (Navy) funds in the amount of $1,839,026 (16%) will be obligated at time of award and will not expire at the end of the current fiscal year. The Naval Sea Systems Command, Washington, D.C., is the contracting activity.</t>
+  </si>
+  <si>
+    <t>General Atomics, San Diego, California, is awarded an $8,837,078 firm-fixed-price order (N0001922F2258) against a previously issued basic ordering agreement (N0001921G0014). This order provides for the development of a two or three launch motor subsystem, two energy storage group tailored configuration of the Electromagnetic Aircraft Launch System (EMALS) and a three wire, six energy absorber subsystem Advanced Arresting Gear System configuration that are compatible with the government of France’s future aircraft carrier and provides acceptable mission capability. Work will be performed in San Diego, California (98.85%); and Tupelo, Mississippi (1.15%), and is expected to be completed in June 2023. Foreign Military Sales customer funds in the amount of $8,837,078 will be obligated at the time of award, none of which will expire at the end of the current fiscal year. The Naval Air Systems Command, Patuxent River, Maryland, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>The Johns Hopkins University Applied Physics Laboratory, Laurel, Maryland, is awarded a $4,396,000,000 cost-plus-fixed-fee, indefinite-delivery/indefinite-quantity contract for research, development, engineering, and test and evaluation for programs throughout the Department of Defense within its core competency areas including strategic systems test and evaluation; submarine security and survivability; space science and engineering; combat systems and guided missiles; air and missile defense and power projection; information technology, simulation, modeling, and operations analysis; and mission related research, development, test and evaluation. This contract includes options which, if exercised, would bring the cumulative value of this contract to $10,600,000,000. Work will be performed in Laurel, Maryland, and is expected to be completed by August 2027. If all options are exercised, work will continue through August 2032. Fiscal 2022 research, development, test and evaluation (Navy) funds in the amount of $6,803,376 will be obligated at time of award and will not expire at the end of the current fiscal year. This contract was not competitively procured in accordance with 10 U.S. Code 2304(c)(3)(B), as implemented in Defense Federal Acquisition Regulation 6.302-3 — industrial mobilization; engineering, developmental, or research capability; or expert services. The Naval Sea Systems Command, Washington, D.C., is the contracting activity (N00024-22-D-6404).</t>
+  </si>
+  <si>
+    <t>BAE Systems Land &amp; Armaments L.P., Sterling Heights, Michigan, was awarded a $278,182,786 firm-fixed-price contract for production units, spare parts and contractor logistics support for the Cold Weather All-Terrain Vehicle. Bids were solicited via the internet with two received. Work locations and funding will be determined with each order, with an estimated completion date of Aug. 19, 2029. U.S. Army Contracting Command, Detroit Arsenal, Michigan, is the contracting activity (W56HZV-22-D-0082).</t>
+  </si>
+  <si>
+    <t>Day and Zimmermann Inc., Parsons, Kansas (W52P1J-22-D-0031); and General Dynamics Ordnance and Tactical Systems Canada Inc., Repentigny, Quebec, Canada (W52P1J-22-D-0032), will compete for each order of the $372,589,589 firm-fixed-price contract to load, assemble and package high-explosive mortar cartridges. Bids were solicited via the internet with three received. Work locations and funding will be determined with each order, with an estimated completion date of Aug. 18, 2027. U.S. Army Contracting Command, Rock Island Arsenal, Illinois, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Oshkosh Defense LLC, Oshkosh, Wisconsin, was awarded a $22,639,245 modification (P00315) to contract W56HZV-20-C-0050 to exercise available options to support the fielding of Joint Light Tactical Vehicles, packaged and installed kits, and trailers. Work will be performed in Oshkosh, Wisconsin, with an estimated completion date of Sept. 30, 2024. Fiscal 2020 other procurement, Army funds and fiscal 2020 and 2022 Marine Corps procurement funds in the amount of $22,639,245 were obligated at the time of the award. U.S. Army Contracting Command, Detroit Arsenal, Michigan, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Advanced Systems and Software Engineering Technologies LLC,* Ridgecrest, California, is awarded a $292,310,598 cost-plus-fixed-fee, cost reimbursable, indefinite-delivery/indefinite-quantity contract. This contract provides system engineering, analysis, research, development, logistics, configuration and data management services in support of the Naval Air Warfare Center Weapons Division’s aircraft integrated product teams for the development, integration, test, evaluation, and fielding of new and upgraded capabilities to Navy aircraft, to include F/A-18, EA-18G, F-35, AV-8B, AH-1/UH-1 aircraft and unmanned aerial systems. Work will be performed in China Lake, California (86.5%); Eglin Air Force Base, Florida (7%); Ridgecrest, California (5%); Point Mugu, California (1%); and various locations within the continental U.S. (0.5%), and is expected to be completed in October 2027. No funds will be obligated at the time of award; funds will be obligated on individual orders as they are issued.  This contract was competitively procured as a small business set-aside; three offers were received. The Naval Air Warfare Center Weapons Division, China Lake, California, is the contracting activity (N6893622D0038).</t>
+  </si>
+  <si>
+    <t>Lockheed Martin Rotary and Mission Systems, Manassas, Virginia, is awarded a $78,423,685 cost-plus-incentive-fee and cost reimbursement contract modification to previously awarded contract N00024-17-C-6259 to exercise options for engineering design and development.  Work will be performed in Manassas, Virginia (65%); Clearwater, Florida (32%); Syracuse, New York (2%); and Marion, Florida (1%), and is expected to be completed by December 2023. Fiscal 2022 other procurement (Navy) funds in the amount of $58,919 will be obligated at time of award, and will not expire at the end of the current fiscal year. The Naval Sea Systems Command, Washington Navy Yard, Washington, D.C., is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Lockheed Martin Corp., Rotary and Mission Systems, Moorestown, New Jersey, is awarded a $13,542,835 cost-plus-incentive-fee modification to previously awarded contract N00024-13-C-5116 for AEGIS combat system engineering agent efforts, which include the design, development, integration, test and delivery of Advanced Capability Build 20. Work will be performed in Moorestown, New Jersey, and is expected to be completed by May 2023. Fiscal 2019 shipbuilding and conversion (Navy) funds in the amount of $7,220,634 (53%); fiscal 2018 shipbuilding and conversion (Navy) funds in the amount of $5,883,043 (44%); and fiscal 2021 shipbuilding and conversion (Navy) funds in the amount of $439,158 (3%) will be obligated at time of award and do not expire at the end of the current fiscal year. The Naval Sea Systems Command, Washington, D.C., is the contracting activity.</t>
+  </si>
+  <si>
+    <t>AM General LLC, South Bend, Indiana, was awarded a $732,741,016 modification (P00042) to contract W56HZV-17-D-0071 for production of High Mobility Multipurpose Wheeled Vehicle Expanded Capacity Vehicle variants. Bids were solicited via the internet with one received. Work locations and funding will be determined with each order, with an estimated completion date of Dec. 31, 2024. U.S. Army Contracting Command, Detroit Arsenal, Michigan, is the contracting activity. (Awarded Aug. 19, 2022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAE Systems Land &amp; Armaments L.P., York, Pennsylvania, was awarded a $49,689,943 cost-no-fee contract for Bradley Fighting Vehicles. Bids were solicited via the internet with one received. Work will be performed in York, Pennsylvania, with an estimated completion date of Aug. 23, 2023. Fiscal 2022 weapons and tracked combat vehicle procurement, Army funds in the amount of $49,689,943 were obligated at the time of the award. U.S. Army Contracting Command, Detroit Arsenal, Michigan, is the contracting activity (W56HZV-22-F-0413). </t>
+  </si>
+  <si>
+    <t>Charles Reed Knight Jr., doing business as Knight's Armament Co.,* Titusville, Florida, was awarded a $14,998,849 modification (P00004) to contract W15QKN-20-D-0044 for the M110 Semi-Automatic Sniper System and various M110 configurations. Bids were solicited via the internet with one received. Work locations and funding will be determined with each order, with an estimated completion date of Sept. 25, 2025. U.S. Army Contracting Command, Newark, New Jersey, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>L-3 Communication Integrated Systems L.P., Greenville, Texas, has been awarded a $96,538,833 cost-plus-fixed-fee and firm-fixed-price contract action for the procurement and fabrication of Group B Ground and System Integration Lab material. Work will be performed in Greenville, Texas, and is expected be complete by June 30, 2024. This contract involved 100% foreign military sales. This award is the result of a sole source acquisition. Foreign Military Sales funds in the amount of $96,538,833 are being obligated at the time of award. The 645th Aeronautical Systems Group, Wright-Patterson Air Force Base, Ohio, is the contracting activity (FA8620-21-G-4027 / FA8620-22-F-4831).</t>
+  </si>
+  <si>
+    <t>Dyncorp International LLC, Fort Worth, Texas, is awarded a $30,268,759 firm-fixed-price, cost-plus-fixed-fee, cost reimbursable modification (P00071) to a previously awarded contract (N6893617C0052). This modification exercises an option to extend services to provide continued organizational level aircraft maintenance and logistics support for aircrew systems and subsystems, search and rescue equipment, and support equipment for the P-3 Orion, C-130 Hercules, F/A-18 Hornet, E/A-18 Growler, AV-8B Harrier II, H-60 Seahawk, and E-2D Hawkeye aircraft in support of the Naval Air Warfare Center Weapons Division (NAWCWD) Naval Test Wing Pacific. Work will be performed in China Lake, California (60%); Point Mugu, California (30 %); Hickam Air Force Base, Hawaii (2%); Lemoore, California (2%); Patrick AFB, Florida (1%); Holloman AFB, New Mexico (1%); Patuxent River, Maryland, (1%); Yuma, Arizona (1%); Miramar, California (1%); and North Island, California (1%), and is expected to be completed in April 2023. Working capital (Navy) funds in the amount of $10,113,024 will be obligated at time of award, none of which will expire at the end of the current fiscal year. The NAWCWD, Point Mugu, California, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Grove U.S. LLC, Shady Grove, Pennsylvania, has been awarded a maximum $266,866,453 fixed-price with economic-price-adjustment, indefinite-delivery requirements contract for commercial cranes. This was a competitive acquisition with one response received. This is a five-year contract with no option periods. Other contracts are expected to be awarded under this solicitation (SPE8EC-21-R-0003) and awardees will compete for a portion of the maximum dollar value. The ordering period end date is Aug. 23, 2027. Using military services are Army, Navy and Marine Corps. Type of appropriation is fiscal 2022 through 2027 defense working capital funds. The contracting activity is the Defense Logistics Agency Troop Support, Philadelphia, Pennsylvania (SPE8EC-22-D-0011).</t>
+  </si>
+  <si>
+    <t>General Dynamics Land Systems Inc., Sterling Heights, Michigan, was awarded a $25,999,349 modification (P00015) to contract W56HZV-22-C-0012 for Abrams systems technical support. Work will be performed in Sterling Heights, Michigan, with an estimated completion date of Sept. 30, 2025. Fiscal 2020 other procurement, Army funds in the amount of $25,999,349 were obligated at the time of the award. U.S. Army Contracting Command, Detroit Arsenal, Michigan, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Raytheon Co., Poulsbo, Washington, is awarded an $18,543,264 cost-plus-fixed-fee and firm-fixed-price, indefinite delivery/indefinite-quantity requirements contract for depot-level support, maintenance and modifications support of the AN/AQS-20 Sonar Mine Detecting Set, and the AN/MHP-20 Deploy and Retrieve system for the AN/AQS-20 System. The AN/AQS-20 is a towed, mine hunting and identification system for Program Executive Office, Unmanned and Small Combatants. This contract includes options which, if exercised, would bring the cumulative value of this contract to $91,706,089. Work will be performed in Portsmouth, Rhode Island (65%); Poulsbo, Washington (30%); and Panama City, Florida (5%); and is expected to be completed by August 2023. If all options are exercised, work will continue through August 2027. No funding will be obligated at time of award. This contract was not competitively procured in accordance with Defense Federal Acquisition Regulation 6.302-1(a)(2)(ii) and (iii) – circumstances permitting other than full and open competition when only one source and no supplies or services will satisfy agency requirements. Naval Surface Warfare Center, Panama City Division, Panama City, Florida, is the contracting activity (N6133122D0004).</t>
+  </si>
+  <si>
+    <t>ATAP Inc., Eastaboga, Alabama (FA8517-22-D-0009); Boneal Inc., Means, Kentucky (FA8517-22-D-0012); and F3 Logistics LLC, Warner Robins, Georgia (FA8517-22-D-0013), have been awarded a multiple award, small business set-aside contract ceiling of $533,500,000 for the sourcing of support equipment (SE) with a unit price of $50,000, or less. This contract provides for the sourcing, acquiring, and delivery of a broad range of ground and aircraft SE items. Work will be performed at various locations, and is expected to be complete by Aug. 25, 2032. This contract involves Army, Navy and Foreign Military Sales to be determined as needed on individual delivery orders. This award is the result of a competitive acquisition with one solicitation posted to sam.gov and nine offers were received. Fiscal 2020 Air Force procurement funds in the amount of $13,646; and fiscal 2021 Air Force procurement funds in the amount of $16,597 are being obligated at the time of award. Air Force Sustainment Center, Robins Air Force Base, Georgia, is the contract activity.</t>
+  </si>
+  <si>
+    <t>Altamira Technologies Corp., McLean, Virginia, has been awarded a $280,000,000 modification (P00029) to a previously awarded, cost-plus-fixed-fee, firm-fixed-price, and cost-plus-incentive-fee, multiple award, indefinite-delivery/indefinite-quantity contract (FA8604-15-D-7977). The contract provides for Advanced Technical Exploitation Program II support for geospatial intelligence (GEOINT) research and development; and measurement and signature intelligence (MASINT) research and development; GEOINT and MASINT operational production support; and other mission areas. Work will be performed at the National Air and Space Intelligence Center, Wright-Patterson Air Force Base, Ohio, and other locations, and is expected to be completed by Oct. 2, 2024. The contract modification provides for an increase to the overall ceiling of the contract; and an extension of the ordering period by one year. This modification increases the estimated contract value from $960,000,000 to $1,240,000,000. Total cumulative face value of the contract is $1,240,000,000. No funds will be obligated at the time of award. Air Force Life Cycle Management Center, Wright-Patterson AFB, Ohio, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Radiance Technologies, Huntsville, Alabama, has been awarded a $280,000,000 modification (P00025) to a previously awarded, cost-plus-fixed-fee, firm-fixed-price, and cost-plus-incentive-fee, multiple award, indefinite-delivery/indefinite-quantity contract (FA8604-15-D-7976). The contract provides for Advanced Technical Exploitation Program II support for geospatial intelligence (GEOINT) research and development; and measurement and signature intelligence (MASINT) research and development; GEOINT and MASINT operational production support; and other mission areas. Work will be performed at the National Air and Space Intelligence Center, Wright-Patterson Air Force Base, Ohio, and other locations,  and is expected to be completed by Oct. 2, 2024. The contract modification provides for an increase to the overall ceiling of the contract; and an extension of the ordering period by one year. This modification increases the estimated contract value from $960,000,000 to $1,240,000,000. Total cumulative face value of the contract is $1,240,000,000. No funds will be obligated at the time of award. Air Force Life Cycle Management Center, Wright-Patterson AFB, Ohio, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Centauri LLC, Chantilly, Virginia, has been awarded a $280,000,000 modification (P00031) to a previously awarded, cost-plus-fixed-fee, firm-fixed-price, and cost-plus-incentive-fee, multiple award, indefinite-delivery/indefinite-quantity contract (FA8604-15-D-7975). The contract provides for Advanced Technical Exploitation Program II support for geospatial intelligence (GEOINT) research and development; and measurement and signature intelligence (MASINT) research and development; GEOINT and MASINT operational production support; and other mission areas. Work will be performed at the National Air and Space Intelligence Center, Wright-Patterson Air Force Base, Ohio, and other locations, and is expected to be completed by Oct. 2, 2024. The contract modification provides for an increase to the overall ceiling of the contract; and an extension of the ordering period by one year. This modification increases the estimated contract value from $960,000,000 to $1,240,000,000. Total cumulative face value of the contract is $1,240,000,000. No funds will be obligated at the time of award. Air Force Life Cycle Management Center, Wright-Patterson AFB, Ohio, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Lockheed Martin Corp., Orlando, Florida, has been awarded a $15,000,000 firm-fixed-price contract for Stand-in Attack Weapon Phase 1.2. This contract provides for all activities associated with the statement of objectives as well as the contractor's proposal for Phase 1.2. Work will be performed in Orlando, Florida, and is expected to be complete by Feb. 25, 2023. This award is the result of a sole source acquisition. Fiscal 2022 Air Force research and development funds in the amount of $15,000,000 are being obligated at the time of award. Air Force Life Cycle Management Center, Eglin Air Force Base, Florida, is the contracting activity (FA8656-22-F-1036).</t>
+  </si>
+  <si>
+    <t>Northrop Grumman Systems Corp., Northridge, California, has been awarded a $15,000,000 firm-fixed-price contract for Stand-in Attack Weapon Phase 1.2. This contract provides for all activities associated with the statement of objectives as well as the contractor's proposal for Phase 1.2. Work will be performed in Northridge, California, and is expected to be complete by Feb. 25, 2023. This award is the result of a sole source acquisition. Fiscal 2022 Air Force research and development funds in the amount of $15,000,000 are being obligated at the time of award. Air Force Life Cycle Management Center, Eglin Air Force Base, Florida, is the contracting activity (FA8656-22-F-1051).</t>
+  </si>
+  <si>
+    <t>L3Harris Mustang Technology Group LP, Plano, Texas, has been awarded a $14,579,829 firm-fixed-price contract for Stand-in Attack Weapon Phase 1.2. This contract provides for all activities associated with the statement of objectives as well as the contractor's proposal for Phase 1.2. Work will be performed in Plano, Texas, and is expected to be complete by Feb. 25, 2023. This award is the result of a sole source acquisition. Fiscal 2022 Air Force research and development funds in the amount of $14,579,829 are being obligated at the time of award. Air Force Life Cycle Management Center, Eglin Air Force Base, Florida, is the contracting activity (FA8656-22-F-1031).</t>
+  </si>
+  <si>
+    <t>Raytheon Missiles and Defense, Tucson, Arizona, has been awarded a non-competitive, firm-fixed-price modification (P00021) to previously awarded contract (FA8675-21-C-0034) in the amount of $8,837,522 for Advanced Medium Range Air-to-Air Missile Production Lot 35 Rectifier Filter Assembly Captive Air Training Missile Retrofit effort. Work will be performed in Tucson, Arizona, and is expected to be completed by May 30, 2026. Fiscal 2021 Air Force missile procurement funds in the amount of $4,485,281; fiscal 2021 Navy weapons procurement funds in the amount of $3,865,690; and Foreign Military Sales funds in the amount of $486,551 are being obligated at the time of award. Air Force Life Cycle Management Center, Air Dominance Division Contracting Office, Eglin Air Force Base, Florida, is the contracting activity.</t>
+  </si>
+  <si>
+    <t>Raytheon Co., Tewksbury, Massachusetts, was awarded a $182,295,333 firm-fixed-price contract for the procurement of National Advanced Surface-to-Air Missile Systems. Bids were solicited via the internet with one received. Work will be performed in Tewksbury, Massachusetts, with an estimated completion date of Aug. 23, 2024. Fiscal 2022 Ukraine Security Assistance Initiative funds in the amount of $182,295,333 were obligated at the time of the award. U.S. Army Contracting Command, Redstone Arsenal, Alabama, is the contracting activity (W31P4Q-22-C-0068).</t>
+  </si>
+  <si>
+    <t>MORSECORP Inc., Cambridge, Massachusetts, was awarded a $44,890,537 firm-fixed-price contract for advanced test and evaluation of artificial intelligence and machine learning progress algorithms. Bids were solicited via the internet with 999 received. Work will be performed in Cambridge, Massachusetts, with an estimated completion date of Aug. 31, 2025. Fiscal 2022 research, development, test, and evaluation, Army funds in the amount of $3,195,693 were obligated at the time of the award. U.S. Army Contracting Command, Aberdeen Proving Ground, Maryland, is the contracting activity (W911QX-22-C-0029).</t>
+  </si>
+  <si>
     <t>https://www.war.gov/News/Contracts/Contract/Article/3134553/</t>
   </si>
   <si>
-    <t>BAE Systems - Norfolk Ship Repair, Norfolk, Virginia, is awarded a $107,736,087, firm-fixed-price contract for the execution of the USS Ross (DDG 71) fiscal 2023 extended dry-docking selected restricted availability. This availability will include a combination of maintenance, modernization and repair of the USS Ross. This contract includes options which, if exercised, would bring the cumulative value of this contract to $123,876,183. Work will be performed in Norfolk, Virginia, and is expected to be completed by March 2024. Fiscal 2022 operations and maintenance (Navy) funds in the amount of $93,897,036 (87%); and fiscal 2022 other procurement (Navy) funds in the amount of $13,839,051 (13%) will be obligated at time of award, of which $93,897,036 will expire at the end of the current fiscal year. This contract was competitively procured using full and open competition via the System for Award Management website. Competitive proposals were received in response to Solicitation Number (N00024-22-R-4422). The Naval Sea Systems Command, Washington, D.C., is the contracting activity (N00024-22-C-4422).</t>
+    <t>https://www.war.gov/News/Contracts/Contract/Article/3136011/</t>
+  </si>
+  <si>
+    <t>https://www.war.gov/News/Contracts/Contract/Article/3137139/</t>
+  </si>
+  <si>
+    <t>https://www.war.gov/News/Contracts/Contract/Article/3138645/</t>
+  </si>
+  <si>
+    <t>https://www.war.gov/News/Contracts/Contract/Article/3140102/</t>
+  </si>
+  <si>
+    <t>https://www.war.gov/News/Contracts/Contract/Article/3141819/</t>
   </si>
 </sst>
 </file>
@@ -124,11 +226,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -472,20 +574,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32A2EF0-6AE5-4C15-9CF0-4CEB2FFB30C8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.9140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,15 +598,334 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1">
         <v>44792</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44792</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44795</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44795</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44796</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44796</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44796</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44796</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44796</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2">
+        <v>44797</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44797</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44797</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44797</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44797</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44798</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44798</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44798</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44799</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>